<commit_message>
Execution, Decode, write back
</commit_message>
<xml_diff>
--- a/OpCodes for Ctrl.xlsx
+++ b/OpCodes for Ctrl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\potts\Documents\GitHub\Project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A89C70-9F0F-49D5-8D2E-E3776CF95767}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA521E6F-4D75-4626-B471-29A57BD42004}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{C3EF1FD4-0928-4246-9FA0-6A46EB4447AA}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>Shift Left Logical</t>
   </si>
@@ -201,8 +201,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -236,10 +244,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B566E783-A5BE-491B-8F0A-3056E12FEEBB}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +574,7 @@
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="D1" s="2" t="s">
         <v>46</v>
       </c>
@@ -579,7 +588,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -593,8 +602,9 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -608,8 +618,26 @@
       <c r="E3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -623,8 +651,26 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -638,8 +684,26 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -653,8 +717,26 @@
       <c r="E6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -668,8 +750,26 @@
       <c r="E7" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -683,8 +783,26 @@
       <c r="E8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -699,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -714,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -733,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -751,8 +869,9 @@
       <c r="G12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -770,8 +889,11 @@
       <c r="G13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -789,8 +911,9 @@
       <c r="G14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -801,8 +924,14 @@
         <v>1</v>
       </c>
       <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -813,6 +942,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="2"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -825,6 +958,9 @@
         <v>1</v>
       </c>
       <c r="E17" s="2"/>
+      <c r="H17" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -837,6 +973,9 @@
         <v>1</v>
       </c>
       <c r="E18" s="2"/>
+      <c r="H18" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -891,8 +1030,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22">
+      <c r="E22" s="2">
         <v>1</v>
       </c>
     </row>
@@ -904,8 +1042,7 @@
         <v>39</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23">
+      <c r="E23" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>